<commit_message>
Atualização do teste 32/10
</commit_message>
<xml_diff>
--- a/Algoritmo_Rota/Planilhas/A_Estrela_Euclidiano/PLN_32_10.xlsx
+++ b/Algoritmo_Rota/Planilhas/A_Estrela_Euclidiano/PLN_32_10.xlsx
@@ -462,7 +462,7 @@
         <v>2098</v>
       </c>
       <c r="E2" t="n">
-        <v>0.03518081506093343</v>
+        <v>0.03041600386301676</v>
       </c>
     </row>
     <row r="3">
@@ -479,7 +479,7 @@
         <v>2165</v>
       </c>
       <c r="E3" t="n">
-        <v>0.03596404393513997</v>
+        <v>0.02858764330546061</v>
       </c>
     </row>
     <row r="4">
@@ -496,7 +496,7 @@
         <v>1784</v>
       </c>
       <c r="E4" t="n">
-        <v>0.04211782614390056</v>
+        <v>0.03171764214833577</v>
       </c>
     </row>
     <row r="5">
@@ -513,7 +513,7 @@
         <v>2199</v>
       </c>
       <c r="E5" t="n">
-        <v>0.03972384929656982</v>
+        <v>0.03155186971028646</v>
       </c>
     </row>
     <row r="6">
@@ -530,7 +530,7 @@
         <v>1768</v>
       </c>
       <c r="E6" t="n">
-        <v>0.03719279766082764</v>
+        <v>0.03110279242197673</v>
       </c>
     </row>
     <row r="7">
@@ -547,7 +547,7 @@
         <v>2051</v>
       </c>
       <c r="E7" t="n">
-        <v>0.03582545916239421</v>
+        <v>0.03106932640075684</v>
       </c>
     </row>
     <row r="8">
@@ -564,7 +564,7 @@
         <v>2136</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0369130293528239</v>
+        <v>0.03144137064615885</v>
       </c>
     </row>
     <row r="9">
@@ -581,7 +581,7 @@
         <v>2100</v>
       </c>
       <c r="E9" t="n">
-        <v>0.03914109071095784</v>
+        <v>0.03159577846527099</v>
       </c>
     </row>
     <row r="10">
@@ -598,7 +598,7 @@
         <v>2267</v>
       </c>
       <c r="E10" t="n">
-        <v>0.03696901003519694</v>
+        <v>0.02847739855448405</v>
       </c>
     </row>
     <row r="11">
@@ -615,7 +615,7 @@
         <v>1938</v>
       </c>
       <c r="E11" t="n">
-        <v>0.03594632148742676</v>
+        <v>0.02911403179168701</v>
       </c>
     </row>
   </sheetData>

</xml_diff>